<commit_message>
Removed modified EFGs from Lacustrine crosswalk.
</commit_message>
<xml_diff>
--- a/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx
+++ b/crosswalks/Geofabric-IUCNGET/Lacustrine-IUCNGET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ecosystem-typology\crosswalks\Geofabric-IUCNGET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\Geofabric-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9D1290-E596-48C4-BD2A-7FFE0FE97079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA51F15-2001-44B9-A35F-F5AF8FBC4CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="990" yWindow="3480" windowWidth="23925" windowHeight="10815" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="60">
   <si>
     <t>semapv:ManualMappingCuration</t>
   </si>
@@ -171,21 +171,6 @@
     <t>F3.5 Canals, ditches and drains</t>
   </si>
   <si>
-    <t>get:groups/F3.1</t>
-  </si>
-  <si>
-    <t>get:groups/F3.2</t>
-  </si>
-  <si>
-    <t>get:groups/F3.3</t>
-  </si>
-  <si>
-    <t>get:groups/F3.4</t>
-  </si>
-  <si>
-    <t>get:groups/F3.5</t>
-  </si>
-  <si>
     <t>F2.4 Freeze-thaw freshwater lakes</t>
   </si>
   <si>
@@ -226,6 +211,12 @@
   </si>
   <si>
     <t>lake: https://w3id.org/env/neap/lakes/</t>
+  </si>
+  <si>
+    <t>owl:Nothing</t>
+  </si>
+  <si>
+    <t>Unclassified</t>
   </si>
 </sst>
 </file>
@@ -319,7 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,6 +323,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,9 +345,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -391,7 +385,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -497,7 +491,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -639,7 +633,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -649,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DD23B2-5C24-4E92-A3A3-39F13C78738A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A1:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -660,42 +654,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -707,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +843,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" ref="A3:A16" si="1">_xlfn.CONCAT("lake:",LEFT(B4,FIND(" ",B4)-1))</f>
+        <f t="shared" ref="A4:A16" si="1">_xlfn.CONCAT("lake:",LEFT(B4,FIND(" ",B4)-1))</f>
         <v>lake:F2.3</v>
       </c>
       <c r="B4" t="s">
@@ -890,16 +884,16 @@
         <v>lake:F2.4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>0</v>
@@ -1075,16 +1069,16 @@
         <v>lake:F2.9</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>0</v>
@@ -1112,16 +1106,16 @@
         <v>lake:F2.10</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>0</v>
@@ -1154,11 +1148,11 @@
       <c r="C12" t="s">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>39</v>
+      <c r="D12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>0</v>
@@ -1191,11 +1185,11 @@
       <c r="C13" t="s">
         <v>1</v>
       </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
+      <c r="D13" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>0</v>
@@ -1228,11 +1222,11 @@
       <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" t="s">
-        <v>41</v>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>0</v>
@@ -1265,11 +1259,11 @@
       <c r="C15" t="s">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
+      <c r="D15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>0</v>
@@ -1302,11 +1296,11 @@
       <c r="C16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" t="s">
-        <v>43</v>
+      <c r="D16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>0</v>
@@ -1398,6 +1392,65 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100772FA3DF59B7CE49A6C16870444FDBEA" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1badbe4fae1da33fa4f3d33d98841982">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e444dda-df07-4069-8b25-4dfb1c3da75a" xmlns:ns3="72d9be16-af35-44ba-8991-a3db737bf75a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35b20e6642ad5eb13a26fdf3049cd990" ns2:_="" ns3:_="">
     <xsd:import namespace="9e444dda-df07-4069-8b25-4dfb1c3da75a"/>
@@ -1673,65 +1726,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D487604F-0564-4158-A24A-3D7190C5619F}">
   <ds:schemaRefs>
@@ -1744,6 +1738,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{66326C79-A0D3-4EA9-86BB-19E204621547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1760,20 +1770,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39241E02-8637-4EBB-8C9C-3CF779AD8349}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC5D47B6-1317-4F93-BD6E-FCBD1047334E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>